<commit_message>
库表修改，实验安排 Signed-off-by: LuoJhno <540088249@qq.com>
</commit_message>
<xml_diff>
--- a/毕业设计相关/数据库设计/实验教学平台_数据字典.xlsx
+++ b/毕业设计相关/数据库设计/实验教学平台_数据字典.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19770" windowHeight="8505"/>
+    <workbookView windowWidth="20385" windowHeight="8085"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186">
   <si>
     <t>实验教学管理平台_数据库表及字段</t>
   </si>
@@ -234,6 +234,21 @@
     <t>课程地点</t>
   </si>
   <si>
+    <t>CSY068</t>
+  </si>
+  <si>
+    <t>备注</t>
+  </si>
+  <si>
+    <t>CSY069</t>
+  </si>
+  <si>
+    <t>CSY06A</t>
+  </si>
+  <si>
+    <t>课程代码</t>
+  </si>
+  <si>
     <t>CSY067</t>
   </si>
   <si>
@@ -415,9 +430,6 @@
   </si>
   <si>
     <t>CSY123</t>
-  </si>
-  <si>
-    <t>备注</t>
   </si>
   <si>
     <t>CSY124</t>
@@ -569,10 +581,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -590,16 +602,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -621,38 +633,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -680,7 +663,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -696,7 +687,37 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -718,17 +739,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -749,13 +761,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -767,13 +923,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -785,151 +935,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -967,15 +979,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -993,9 +996,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1015,17 +1020,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1040,6 +1034,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -1048,10 +1060,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1060,133 +1072,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1547,10 +1559,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:K128"/>
+  <dimension ref="A1:K131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A116" workbookViewId="0">
-      <selection activeCell="D128" sqref="D128"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -2147,159 +2159,159 @@
         <v>72</v>
       </c>
       <c r="C47" t="s">
-        <v>8</v>
+        <v>70</v>
       </c>
       <c r="D47" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" s="1"/>
+      <c r="B48" t="s">
+        <v>74</v>
+      </c>
+      <c r="C48" t="s">
+        <v>37</v>
+      </c>
+      <c r="D48" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" s="1"/>
+      <c r="B49" t="s">
+        <v>75</v>
+      </c>
+      <c r="C49" t="s">
+        <v>37</v>
+      </c>
+      <c r="D49" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" s="1"/>
+      <c r="B50" t="s">
+        <v>77</v>
+      </c>
+      <c r="C50" t="s">
+        <v>66</v>
+      </c>
+      <c r="D50" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="48" spans="1:11">
-      <c r="A48" s="3"/>
-      <c r="B48" s="3"/>
-      <c r="C48" s="3"/>
-      <c r="D48" s="3"/>
-      <c r="E48" s="3"/>
-      <c r="F48" s="3"/>
-      <c r="G48" s="3"/>
-      <c r="H48" s="3"/>
-      <c r="I48" s="3"/>
-      <c r="J48" s="3"/>
-      <c r="K48" s="3"/>
-    </row>
-    <row r="49" spans="1:11">
-      <c r="A49" s="3"/>
-      <c r="B49" s="3"/>
-      <c r="C49" s="3"/>
-      <c r="D49" s="3"/>
-      <c r="E49" s="3"/>
-      <c r="F49" s="3"/>
-      <c r="G49" s="3"/>
-      <c r="H49" s="3"/>
-      <c r="I49" s="3"/>
-      <c r="J49" s="3"/>
-      <c r="K49" s="3"/>
-    </row>
-    <row r="50" spans="1:4">
-      <c r="A50" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="B50" t="s">
+    <row r="51" spans="1:11">
+      <c r="A51" s="3"/>
+      <c r="B51" s="3"/>
+      <c r="C51" s="3"/>
+      <c r="D51" s="3"/>
+      <c r="E51" s="3"/>
+      <c r="F51" s="3"/>
+      <c r="G51" s="3"/>
+      <c r="H51" s="3"/>
+      <c r="I51" s="3"/>
+      <c r="J51" s="3"/>
+      <c r="K51" s="3"/>
+    </row>
+    <row r="52" spans="1:11">
+      <c r="A52" s="3"/>
+      <c r="B52" s="3"/>
+      <c r="C52" s="3"/>
+      <c r="D52" s="3"/>
+      <c r="E52" s="3"/>
+      <c r="F52" s="3"/>
+      <c r="G52" s="3"/>
+      <c r="H52" s="3"/>
+      <c r="I52" s="3"/>
+      <c r="J52" s="3"/>
+      <c r="K52" s="3"/>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B53" t="s">
         <v>40</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C53" t="s">
         <v>12</v>
       </c>
-      <c r="D50" t="s">
+      <c r="D53" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
-      <c r="A51" s="1"/>
-      <c r="B51" t="s">
+    <row r="54" spans="1:4">
+      <c r="A54" s="1"/>
+      <c r="B54" t="s">
         <v>54</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C54" t="s">
         <v>19</v>
       </c>
-      <c r="D51" t="s">
+      <c r="D54" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
-      <c r="A52" s="1"/>
-      <c r="B52" t="s">
-        <v>74</v>
-      </c>
-      <c r="C52" t="s">
+    <row r="55" spans="1:4">
+      <c r="A55" s="1"/>
+      <c r="B55" t="s">
+        <v>79</v>
+      </c>
+      <c r="C55" t="s">
         <v>59</v>
       </c>
-      <c r="D52" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11">
-      <c r="A53" s="3"/>
-      <c r="B53" s="3"/>
-      <c r="C53" s="3"/>
-      <c r="D53" s="3"/>
-      <c r="E53" s="3"/>
-      <c r="F53" s="3"/>
-      <c r="G53" s="3"/>
-      <c r="H53" s="3"/>
-      <c r="I53" s="3"/>
-      <c r="J53" s="3"/>
-      <c r="K53" s="3"/>
-    </row>
-    <row r="54" spans="1:11">
-      <c r="A54" s="3"/>
-      <c r="B54" s="3"/>
-      <c r="C54" s="3"/>
-      <c r="D54" s="3"/>
-      <c r="E54" s="3"/>
-      <c r="F54" s="3"/>
-      <c r="G54" s="3"/>
-      <c r="H54" s="3"/>
-      <c r="I54" s="3"/>
-      <c r="J54" s="3"/>
-      <c r="K54" s="3"/>
-    </row>
-    <row r="55" spans="1:4">
-      <c r="A55" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="B55" t="s">
+      <c r="D55" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11">
+      <c r="A56" s="3"/>
+      <c r="B56" s="3"/>
+      <c r="C56" s="3"/>
+      <c r="D56" s="3"/>
+      <c r="E56" s="3"/>
+      <c r="F56" s="3"/>
+      <c r="G56" s="3"/>
+      <c r="H56" s="3"/>
+      <c r="I56" s="3"/>
+      <c r="J56" s="3"/>
+      <c r="K56" s="3"/>
+    </row>
+    <row r="57" spans="1:11">
+      <c r="A57" s="3"/>
+      <c r="B57" s="3"/>
+      <c r="C57" s="3"/>
+      <c r="D57" s="3"/>
+      <c r="E57" s="3"/>
+      <c r="F57" s="3"/>
+      <c r="G57" s="3"/>
+      <c r="H57" s="3"/>
+      <c r="I57" s="3"/>
+      <c r="J57" s="3"/>
+      <c r="K57" s="3"/>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B58" t="s">
         <v>40</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C58" t="s">
         <v>12</v>
       </c>
-      <c r="D55" t="s">
+      <c r="D58" t="s">
         <v>41</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4">
-      <c r="A56" s="1"/>
-      <c r="B56" t="s">
-        <v>54</v>
-      </c>
-      <c r="C56" t="s">
-        <v>19</v>
-      </c>
-      <c r="D56" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4">
-      <c r="A57" s="1"/>
-      <c r="B57" t="s">
-        <v>78</v>
-      </c>
-      <c r="C57" t="s">
-        <v>19</v>
-      </c>
-      <c r="D57" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4">
-      <c r="A58" s="1"/>
-      <c r="B58" t="s">
-        <v>48</v>
-      </c>
-      <c r="C58" t="s">
-        <v>19</v>
-      </c>
-      <c r="D58" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="59" spans="1:4">
       <c r="A59" s="1"/>
       <c r="B59" t="s">
-        <v>81</v>
+        <v>54</v>
       </c>
       <c r="C59" t="s">
-        <v>70</v>
+        <v>19</v>
       </c>
       <c r="D59" t="s">
         <v>82</v>
@@ -2311,322 +2323,322 @@
         <v>83</v>
       </c>
       <c r="C60" t="s">
+        <v>19</v>
+      </c>
+      <c r="D60" t="s">
         <v>84</v>
-      </c>
-      <c r="D60" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="61" spans="1:4">
       <c r="A61" s="1"/>
       <c r="B61" t="s">
-        <v>86</v>
+        <v>48</v>
       </c>
       <c r="C61" t="s">
-        <v>87</v>
+        <v>19</v>
       </c>
       <c r="D61" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="62" spans="1:4">
       <c r="A62" s="1"/>
       <c r="B62" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C62" t="s">
+        <v>70</v>
+      </c>
+      <c r="D62" t="s">
         <v>87</v>
-      </c>
-      <c r="D62" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="63" spans="1:4">
       <c r="A63" s="1"/>
       <c r="B63" t="s">
+        <v>88</v>
+      </c>
+      <c r="C63" t="s">
+        <v>89</v>
+      </c>
+      <c r="D63" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
+      <c r="A64" s="1"/>
+      <c r="B64" t="s">
         <v>91</v>
       </c>
-      <c r="C63" t="s">
+      <c r="C64" t="s">
+        <v>92</v>
+      </c>
+      <c r="D64" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
+      <c r="A65" s="1"/>
+      <c r="B65" t="s">
+        <v>94</v>
+      </c>
+      <c r="C65" t="s">
+        <v>92</v>
+      </c>
+      <c r="D65" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4">
+      <c r="A66" s="1"/>
+      <c r="B66" t="s">
+        <v>96</v>
+      </c>
+      <c r="C66" t="s">
         <v>66</v>
       </c>
-      <c r="D63" t="s">
+      <c r="D66" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="64" spans="1:11">
-      <c r="A64" s="3"/>
-      <c r="B64" s="3"/>
-      <c r="C64" s="3"/>
-      <c r="D64" s="3"/>
-      <c r="E64" s="3"/>
-      <c r="F64" s="3"/>
-      <c r="G64" s="3"/>
-      <c r="H64" s="3"/>
-      <c r="I64" s="3"/>
-      <c r="J64" s="3"/>
-      <c r="K64" s="3"/>
-    </row>
-    <row r="65" spans="1:11">
-      <c r="A65" s="3"/>
-      <c r="B65" s="3"/>
-      <c r="C65" s="3"/>
-      <c r="D65" s="3"/>
-      <c r="E65" s="3"/>
-      <c r="F65" s="3"/>
-      <c r="G65" s="3"/>
-      <c r="H65" s="3"/>
-      <c r="I65" s="3"/>
-      <c r="J65" s="3"/>
-      <c r="K65" s="3"/>
-    </row>
-    <row r="66" spans="1:4">
-      <c r="A66" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B66" t="s">
+    <row r="67" spans="1:11">
+      <c r="A67" s="3"/>
+      <c r="B67" s="3"/>
+      <c r="C67" s="3"/>
+      <c r="D67" s="3"/>
+      <c r="E67" s="3"/>
+      <c r="F67" s="3"/>
+      <c r="G67" s="3"/>
+      <c r="H67" s="3"/>
+      <c r="I67" s="3"/>
+      <c r="J67" s="3"/>
+      <c r="K67" s="3"/>
+    </row>
+    <row r="68" spans="1:11">
+      <c r="A68" s="3"/>
+      <c r="B68" s="3"/>
+      <c r="C68" s="3"/>
+      <c r="D68" s="3"/>
+      <c r="E68" s="3"/>
+      <c r="F68" s="3"/>
+      <c r="G68" s="3"/>
+      <c r="H68" s="3"/>
+      <c r="I68" s="3"/>
+      <c r="J68" s="3"/>
+      <c r="K68" s="3"/>
+    </row>
+    <row r="69" spans="1:4">
+      <c r="A69" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B69" t="s">
         <v>40</v>
       </c>
-      <c r="C66" t="s">
+      <c r="C69" t="s">
         <v>12</v>
       </c>
-      <c r="D66" t="s">
+      <c r="D69" t="s">
         <v>41</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4">
-      <c r="A67" s="1"/>
-      <c r="B67" t="s">
-        <v>78</v>
-      </c>
-      <c r="C67" t="s">
-        <v>19</v>
-      </c>
-      <c r="D67" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4">
-      <c r="A68" s="1"/>
-      <c r="B68" t="s">
-        <v>93</v>
-      </c>
-      <c r="C68" t="s">
-        <v>94</v>
-      </c>
-      <c r="D68" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4">
-      <c r="A69" s="1"/>
-      <c r="B69" t="s">
-        <v>96</v>
-      </c>
-      <c r="C69" t="s">
-        <v>87</v>
-      </c>
-      <c r="D69" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="70" spans="1:4">
       <c r="A70" s="1"/>
       <c r="B70" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="C70" t="s">
-        <v>99</v>
+        <v>19</v>
       </c>
       <c r="D70" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
     </row>
     <row r="71" spans="1:4">
       <c r="A71" s="1"/>
       <c r="B71" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C71" t="s">
-        <v>70</v>
+        <v>99</v>
       </c>
       <c r="D71" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="72" spans="1:4">
       <c r="A72" s="1"/>
       <c r="B72" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C72" t="s">
-        <v>19</v>
+        <v>92</v>
       </c>
       <c r="D72" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="73" spans="1:4">
       <c r="A73" s="1"/>
       <c r="B73" t="s">
+        <v>103</v>
+      </c>
+      <c r="C73" t="s">
+        <v>104</v>
+      </c>
+      <c r="D73" t="s">
         <v>105</v>
       </c>
-      <c r="C73" t="s">
+    </row>
+    <row r="74" spans="1:4">
+      <c r="A74" s="1"/>
+      <c r="B74" t="s">
+        <v>106</v>
+      </c>
+      <c r="C74" t="s">
+        <v>70</v>
+      </c>
+      <c r="D74" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4">
+      <c r="A75" s="1"/>
+      <c r="B75" t="s">
+        <v>108</v>
+      </c>
+      <c r="C75" t="s">
+        <v>19</v>
+      </c>
+      <c r="D75" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4">
+      <c r="A76" s="1"/>
+      <c r="B76" t="s">
+        <v>110</v>
+      </c>
+      <c r="C76" t="s">
         <v>66</v>
       </c>
-      <c r="D73" t="s">
+      <c r="D76" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="74" spans="1:11">
-      <c r="A74" s="3"/>
-      <c r="B74" s="3"/>
-      <c r="C74" s="3"/>
-      <c r="D74" s="3"/>
-      <c r="E74" s="3"/>
-      <c r="F74" s="3"/>
-      <c r="G74" s="3"/>
-      <c r="H74" s="3"/>
-      <c r="I74" s="3"/>
-      <c r="J74" s="3"/>
-      <c r="K74" s="3"/>
-    </row>
-    <row r="75" spans="1:11">
-      <c r="A75" s="3"/>
-      <c r="B75" s="3"/>
-      <c r="C75" s="3"/>
-      <c r="D75" s="3"/>
-      <c r="E75" s="3"/>
-      <c r="F75" s="3"/>
-      <c r="G75" s="3"/>
-      <c r="H75" s="3"/>
-      <c r="I75" s="3"/>
-      <c r="J75" s="3"/>
-      <c r="K75" s="3"/>
-    </row>
-    <row r="76" spans="1:4">
-      <c r="A76" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="B76" t="s">
-        <v>107</v>
-      </c>
-      <c r="C76" t="s">
+    <row r="77" spans="1:11">
+      <c r="A77" s="3"/>
+      <c r="B77" s="3"/>
+      <c r="C77" s="3"/>
+      <c r="D77" s="3"/>
+      <c r="E77" s="3"/>
+      <c r="F77" s="3"/>
+      <c r="G77" s="3"/>
+      <c r="H77" s="3"/>
+      <c r="I77" s="3"/>
+      <c r="J77" s="3"/>
+      <c r="K77" s="3"/>
+    </row>
+    <row r="78" spans="1:11">
+      <c r="A78" s="3"/>
+      <c r="B78" s="3"/>
+      <c r="C78" s="3"/>
+      <c r="D78" s="3"/>
+      <c r="E78" s="3"/>
+      <c r="F78" s="3"/>
+      <c r="G78" s="3"/>
+      <c r="H78" s="3"/>
+      <c r="I78" s="3"/>
+      <c r="J78" s="3"/>
+      <c r="K78" s="3"/>
+    </row>
+    <row r="79" spans="1:4">
+      <c r="A79" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B79" t="s">
+        <v>112</v>
+      </c>
+      <c r="C79" t="s">
         <v>19</v>
       </c>
-      <c r="D76" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4">
-      <c r="A77" s="1"/>
-      <c r="B77" t="s">
-        <v>109</v>
-      </c>
-      <c r="C77" t="s">
+      <c r="D79" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4">
+      <c r="A80" s="1"/>
+      <c r="B80" t="s">
+        <v>114</v>
+      </c>
+      <c r="C80" t="s">
         <v>37</v>
       </c>
-      <c r="D77" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4">
-      <c r="A78" s="1"/>
-      <c r="B78" t="s">
-        <v>111</v>
-      </c>
-      <c r="C78" t="s">
+      <c r="D80" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4">
+      <c r="A81" s="1"/>
+      <c r="B81" t="s">
+        <v>116</v>
+      </c>
+      <c r="C81" t="s">
         <v>66</v>
       </c>
-      <c r="D78" t="s">
+      <c r="D81" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="79" spans="1:11">
-      <c r="A79" s="3"/>
-      <c r="B79" s="3"/>
-      <c r="C79" s="3"/>
-      <c r="D79" s="3"/>
-      <c r="E79" s="3"/>
-      <c r="F79" s="3"/>
-      <c r="G79" s="3"/>
-      <c r="H79" s="3"/>
-      <c r="I79" s="3"/>
-      <c r="J79" s="3"/>
-      <c r="K79" s="3"/>
-    </row>
-    <row r="80" spans="1:11">
-      <c r="A80" s="3"/>
-      <c r="B80" s="3"/>
-      <c r="C80" s="3"/>
-      <c r="D80" s="3"/>
-      <c r="E80" s="3"/>
-      <c r="F80" s="3"/>
-      <c r="G80" s="3"/>
-      <c r="H80" s="3"/>
-      <c r="I80" s="3"/>
-      <c r="J80" s="3"/>
-      <c r="K80" s="3"/>
-    </row>
-    <row r="81" spans="1:4">
-      <c r="A81" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="B81" t="s">
-        <v>113</v>
-      </c>
-      <c r="C81" t="s">
+    <row r="82" spans="1:11">
+      <c r="A82" s="3"/>
+      <c r="B82" s="3"/>
+      <c r="C82" s="3"/>
+      <c r="D82" s="3"/>
+      <c r="E82" s="3"/>
+      <c r="F82" s="3"/>
+      <c r="G82" s="3"/>
+      <c r="H82" s="3"/>
+      <c r="I82" s="3"/>
+      <c r="J82" s="3"/>
+      <c r="K82" s="3"/>
+    </row>
+    <row r="83" spans="1:11">
+      <c r="A83" s="3"/>
+      <c r="B83" s="3"/>
+      <c r="C83" s="3"/>
+      <c r="D83" s="3"/>
+      <c r="E83" s="3"/>
+      <c r="F83" s="3"/>
+      <c r="G83" s="3"/>
+      <c r="H83" s="3"/>
+      <c r="I83" s="3"/>
+      <c r="J83" s="3"/>
+      <c r="K83" s="3"/>
+    </row>
+    <row r="84" spans="1:4">
+      <c r="A84" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B84" t="s">
+        <v>118</v>
+      </c>
+      <c r="C84" t="s">
         <v>19</v>
       </c>
-      <c r="D81" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4">
-      <c r="A82" s="1"/>
-      <c r="B82" t="s">
-        <v>107</v>
-      </c>
-      <c r="C82" t="s">
-        <v>19</v>
-      </c>
-      <c r="D82" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4">
-      <c r="A83" s="1"/>
-      <c r="B83" t="s">
-        <v>115</v>
-      </c>
-      <c r="C83" t="s">
-        <v>37</v>
-      </c>
-      <c r="D83" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4">
-      <c r="A84" s="1"/>
-      <c r="B84" t="s">
-        <v>117</v>
-      </c>
-      <c r="C84" t="s">
-        <v>37</v>
-      </c>
       <c r="D84" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="85" spans="1:4">
       <c r="A85" s="1"/>
       <c r="B85" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="C85" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="D85" t="s">
-        <v>64</v>
+        <v>113</v>
       </c>
     </row>
     <row r="86" spans="1:4">
@@ -2635,19 +2647,19 @@
         <v>120</v>
       </c>
       <c r="C86" t="s">
-        <v>66</v>
+        <v>37</v>
       </c>
       <c r="D86" t="s">
-        <v>67</v>
+        <v>121</v>
       </c>
     </row>
     <row r="87" spans="1:4">
       <c r="A87" s="1"/>
       <c r="B87" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C87" t="s">
-        <v>122</v>
+        <v>37</v>
       </c>
       <c r="D87" t="s">
         <v>123</v>
@@ -2659,438 +2671,438 @@
         <v>124</v>
       </c>
       <c r="C88" t="s">
+        <v>37</v>
+      </c>
+      <c r="D88" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4">
+      <c r="A89" s="1"/>
+      <c r="B89" t="s">
+        <v>125</v>
+      </c>
+      <c r="C89" t="s">
         <v>66</v>
       </c>
-      <c r="D88" t="s">
+      <c r="D89" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4">
+      <c r="A90" s="1"/>
+      <c r="B90" t="s">
+        <v>126</v>
+      </c>
+      <c r="C90" t="s">
+        <v>127</v>
+      </c>
+      <c r="D90" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4">
+      <c r="A91" s="1"/>
+      <c r="B91" t="s">
+        <v>129</v>
+      </c>
+      <c r="C91" t="s">
+        <v>66</v>
+      </c>
+      <c r="D91" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="89" spans="1:11">
-      <c r="A89" s="3"/>
-      <c r="B89" s="3"/>
-      <c r="C89" s="3"/>
-      <c r="D89" s="3"/>
-      <c r="E89" s="3"/>
-      <c r="F89" s="3"/>
-      <c r="G89" s="3"/>
-      <c r="H89" s="3"/>
-      <c r="I89" s="3"/>
-      <c r="J89" s="3"/>
-      <c r="K89" s="3"/>
-    </row>
-    <row r="90" spans="1:11">
-      <c r="A90" s="3"/>
-      <c r="B90" s="3"/>
-      <c r="C90" s="3"/>
-      <c r="D90" s="3"/>
-      <c r="E90" s="3"/>
-      <c r="F90" s="3"/>
-      <c r="G90" s="3"/>
-      <c r="H90" s="3"/>
-      <c r="I90" s="3"/>
-      <c r="J90" s="3"/>
-      <c r="K90" s="3"/>
-    </row>
-    <row r="91" spans="1:4">
-      <c r="A91" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="B91" t="s">
-        <v>113</v>
-      </c>
-      <c r="C91" t="s">
+    <row r="92" spans="1:11">
+      <c r="A92" s="3"/>
+      <c r="B92" s="3"/>
+      <c r="C92" s="3"/>
+      <c r="D92" s="3"/>
+      <c r="E92" s="3"/>
+      <c r="F92" s="3"/>
+      <c r="G92" s="3"/>
+      <c r="H92" s="3"/>
+      <c r="I92" s="3"/>
+      <c r="J92" s="3"/>
+      <c r="K92" s="3"/>
+    </row>
+    <row r="93" spans="1:11">
+      <c r="A93" s="3"/>
+      <c r="B93" s="3"/>
+      <c r="C93" s="3"/>
+      <c r="D93" s="3"/>
+      <c r="E93" s="3"/>
+      <c r="F93" s="3"/>
+      <c r="G93" s="3"/>
+      <c r="H93" s="3"/>
+      <c r="I93" s="3"/>
+      <c r="J93" s="3"/>
+      <c r="K93" s="3"/>
+    </row>
+    <row r="94" spans="1:4">
+      <c r="A94" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B94" t="s">
+        <v>118</v>
+      </c>
+      <c r="C94" t="s">
         <v>19</v>
       </c>
-      <c r="D91" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4">
-      <c r="A92" s="1"/>
-      <c r="B92" t="s">
-        <v>126</v>
-      </c>
-      <c r="C92" t="s">
-        <v>19</v>
-      </c>
-      <c r="D92" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4">
-      <c r="A93" s="1"/>
-      <c r="B93" t="s">
-        <v>18</v>
-      </c>
-      <c r="C93" t="s">
-        <v>19</v>
-      </c>
-      <c r="D93" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4">
-      <c r="A94" s="1"/>
-      <c r="B94" t="s">
-        <v>128</v>
-      </c>
-      <c r="C94" t="s">
-        <v>87</v>
-      </c>
       <c r="D94" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
     </row>
     <row r="95" spans="1:4">
       <c r="A95" s="1"/>
       <c r="B95" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C95" t="s">
-        <v>70</v>
+        <v>19</v>
       </c>
       <c r="D95" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="96" spans="1:4">
       <c r="A96" s="1"/>
       <c r="B96" t="s">
-        <v>132</v>
+        <v>18</v>
       </c>
       <c r="C96" t="s">
-        <v>99</v>
+        <v>19</v>
       </c>
       <c r="D96" t="s">
-        <v>133</v>
+        <v>33</v>
       </c>
     </row>
     <row r="97" spans="1:4">
       <c r="A97" s="1"/>
       <c r="B97" t="s">
+        <v>133</v>
+      </c>
+      <c r="C97" t="s">
+        <v>92</v>
+      </c>
+      <c r="D97" t="s">
         <v>134</v>
-      </c>
-      <c r="C97" t="s">
-        <v>87</v>
-      </c>
-      <c r="D97" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="98" spans="1:4">
       <c r="A98" s="1"/>
       <c r="B98" t="s">
+        <v>135</v>
+      </c>
+      <c r="C98" t="s">
+        <v>70</v>
+      </c>
+      <c r="D98" t="s">
         <v>136</v>
-      </c>
-      <c r="C98" t="s">
-        <v>66</v>
-      </c>
-      <c r="D98" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="99" spans="1:4">
       <c r="A99" s="1"/>
       <c r="B99" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C99" t="s">
-        <v>87</v>
+        <v>104</v>
       </c>
       <c r="D99" t="s">
-        <v>139</v>
+        <v>73</v>
       </c>
     </row>
     <row r="100" spans="1:4">
       <c r="A100" s="1"/>
       <c r="B100" t="s">
+        <v>138</v>
+      </c>
+      <c r="C100" t="s">
+        <v>92</v>
+      </c>
+      <c r="D100" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4">
+      <c r="A101" s="1"/>
+      <c r="B101" t="s">
         <v>140</v>
       </c>
-      <c r="C100" t="s">
+      <c r="C101" t="s">
         <v>66</v>
       </c>
-      <c r="D100" t="s">
+      <c r="D101" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4">
+      <c r="A102" s="1"/>
+      <c r="B102" t="s">
+        <v>142</v>
+      </c>
+      <c r="C102" t="s">
+        <v>92</v>
+      </c>
+      <c r="D102" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4">
+      <c r="A103" s="1"/>
+      <c r="B103" t="s">
+        <v>144</v>
+      </c>
+      <c r="C103" t="s">
+        <v>66</v>
+      </c>
+      <c r="D103" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="101" spans="1:11">
-      <c r="A101" s="3"/>
-      <c r="B101" s="3"/>
-      <c r="C101" s="3"/>
-      <c r="D101" s="3"/>
-      <c r="E101" s="3"/>
-      <c r="F101" s="3"/>
-      <c r="G101" s="3"/>
-      <c r="H101" s="3"/>
-      <c r="I101" s="3"/>
-      <c r="J101" s="3"/>
-      <c r="K101" s="3"/>
-    </row>
-    <row r="102" spans="1:11">
-      <c r="A102" s="3"/>
-      <c r="B102" s="3"/>
-      <c r="C102" s="3"/>
-      <c r="D102" s="3"/>
-      <c r="E102" s="3"/>
-      <c r="F102" s="3"/>
-      <c r="G102" s="3"/>
-      <c r="H102" s="3"/>
-      <c r="I102" s="3"/>
-      <c r="J102" s="3"/>
-      <c r="K102" s="3"/>
-    </row>
-    <row r="103" spans="1:4">
-      <c r="A103" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="B103" t="s">
-        <v>142</v>
-      </c>
-      <c r="C103" t="s">
+    <row r="104" spans="1:11">
+      <c r="A104" s="3"/>
+      <c r="B104" s="3"/>
+      <c r="C104" s="3"/>
+      <c r="D104" s="3"/>
+      <c r="E104" s="3"/>
+      <c r="F104" s="3"/>
+      <c r="G104" s="3"/>
+      <c r="H104" s="3"/>
+      <c r="I104" s="3"/>
+      <c r="J104" s="3"/>
+      <c r="K104" s="3"/>
+    </row>
+    <row r="105" spans="1:11">
+      <c r="A105" s="3"/>
+      <c r="B105" s="3"/>
+      <c r="C105" s="3"/>
+      <c r="D105" s="3"/>
+      <c r="E105" s="3"/>
+      <c r="F105" s="3"/>
+      <c r="G105" s="3"/>
+      <c r="H105" s="3"/>
+      <c r="I105" s="3"/>
+      <c r="J105" s="3"/>
+      <c r="K105" s="3"/>
+    </row>
+    <row r="106" spans="1:4">
+      <c r="A106" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B106" t="s">
+        <v>146</v>
+      </c>
+      <c r="C106" t="s">
         <v>19</v>
       </c>
-      <c r="D103" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4">
-      <c r="A104" s="1"/>
-      <c r="B104" t="s">
-        <v>144</v>
-      </c>
-      <c r="C104" t="s">
-        <v>37</v>
-      </c>
-      <c r="D104" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4">
-      <c r="A105" s="1"/>
-      <c r="B105" t="s">
-        <v>146</v>
-      </c>
-      <c r="C105" t="s">
-        <v>87</v>
-      </c>
-      <c r="D105" t="s">
+      <c r="D106" t="s">
         <v>147</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4">
-      <c r="A106" s="1"/>
-      <c r="B106" t="s">
-        <v>148</v>
-      </c>
-      <c r="C106" t="s">
-        <v>149</v>
-      </c>
-      <c r="D106" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="107" spans="1:4">
       <c r="A107" s="1"/>
       <c r="B107" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C107" t="s">
-        <v>87</v>
+        <v>37</v>
       </c>
       <c r="D107" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="108" spans="1:4">
       <c r="A108" s="1"/>
       <c r="B108" t="s">
+        <v>150</v>
+      </c>
+      <c r="C108" t="s">
+        <v>92</v>
+      </c>
+      <c r="D108" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4">
+      <c r="A109" s="1"/>
+      <c r="B109" t="s">
+        <v>152</v>
+      </c>
+      <c r="C109" t="s">
         <v>153</v>
       </c>
-      <c r="C108" t="s">
+      <c r="D109" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4">
+      <c r="A110" s="1"/>
+      <c r="B110" t="s">
+        <v>155</v>
+      </c>
+      <c r="C110" t="s">
+        <v>92</v>
+      </c>
+      <c r="D110" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4">
+      <c r="A111" s="1"/>
+      <c r="B111" t="s">
+        <v>157</v>
+      </c>
+      <c r="C111" t="s">
         <v>66</v>
       </c>
-      <c r="D108" t="s">
+      <c r="D111" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="109" spans="1:11">
-      <c r="A109" s="3"/>
-      <c r="B109" s="3"/>
-      <c r="C109" s="3"/>
-      <c r="D109" s="3"/>
-      <c r="E109" s="3"/>
-      <c r="F109" s="3"/>
-      <c r="G109" s="3"/>
-      <c r="H109" s="3"/>
-      <c r="I109" s="3"/>
-      <c r="J109" s="3"/>
-      <c r="K109" s="3"/>
-    </row>
-    <row r="110" spans="1:11">
-      <c r="A110" s="3"/>
-      <c r="B110" s="3"/>
-      <c r="C110" s="3"/>
-      <c r="D110" s="3"/>
-      <c r="E110" s="3"/>
-      <c r="F110" s="3"/>
-      <c r="G110" s="3"/>
-      <c r="H110" s="3"/>
-      <c r="I110" s="3"/>
-      <c r="J110" s="3"/>
-      <c r="K110" s="3"/>
-    </row>
-    <row r="111" spans="1:4">
-      <c r="A111" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="B111" t="s">
+    <row r="112" spans="1:11">
+      <c r="A112" s="3"/>
+      <c r="B112" s="3"/>
+      <c r="C112" s="3"/>
+      <c r="D112" s="3"/>
+      <c r="E112" s="3"/>
+      <c r="F112" s="3"/>
+      <c r="G112" s="3"/>
+      <c r="H112" s="3"/>
+      <c r="I112" s="3"/>
+      <c r="J112" s="3"/>
+      <c r="K112" s="3"/>
+    </row>
+    <row r="113" spans="1:11">
+      <c r="A113" s="3"/>
+      <c r="B113" s="3"/>
+      <c r="C113" s="3"/>
+      <c r="D113" s="3"/>
+      <c r="E113" s="3"/>
+      <c r="F113" s="3"/>
+      <c r="G113" s="3"/>
+      <c r="H113" s="3"/>
+      <c r="I113" s="3"/>
+      <c r="J113" s="3"/>
+      <c r="K113" s="3"/>
+    </row>
+    <row r="114" spans="1:4">
+      <c r="A114" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B114" t="s">
         <v>18</v>
       </c>
-      <c r="C111" t="s">
+      <c r="C114" t="s">
         <v>19</v>
       </c>
-      <c r="D111" t="s">
+      <c r="D114" t="s">
         <v>33</v>
-      </c>
-    </row>
-    <row r="112" spans="1:4">
-      <c r="A112" s="1"/>
-      <c r="B112" t="s">
-        <v>155</v>
-      </c>
-      <c r="C112" t="s">
-        <v>19</v>
-      </c>
-      <c r="D112" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="113" spans="1:4">
-      <c r="A113" s="1"/>
-      <c r="B113" t="s">
-        <v>157</v>
-      </c>
-      <c r="C113" t="s">
-        <v>70</v>
-      </c>
-      <c r="D113" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="114" spans="1:4">
-      <c r="A114" s="1"/>
-      <c r="B114" t="s">
-        <v>159</v>
-      </c>
-      <c r="C114" t="s">
-        <v>70</v>
-      </c>
-      <c r="D114" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="115" spans="1:4">
       <c r="A115" s="1"/>
       <c r="B115" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C115" t="s">
-        <v>94</v>
+        <v>19</v>
       </c>
       <c r="D115" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="116" spans="1:4">
       <c r="A116" s="1"/>
       <c r="B116" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C116" t="s">
-        <v>99</v>
+        <v>70</v>
       </c>
       <c r="D116" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="117" spans="1:4">
       <c r="A117" s="1"/>
       <c r="B117" t="s">
+        <v>163</v>
+      </c>
+      <c r="C117" t="s">
+        <v>70</v>
+      </c>
+      <c r="D117" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4">
+      <c r="A118" s="1"/>
+      <c r="B118" t="s">
         <v>165</v>
       </c>
-      <c r="C117" t="s">
+      <c r="C118" t="s">
+        <v>99</v>
+      </c>
+      <c r="D118" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4">
+      <c r="A119" s="1"/>
+      <c r="B119" t="s">
+        <v>167</v>
+      </c>
+      <c r="C119" t="s">
+        <v>104</v>
+      </c>
+      <c r="D119" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4">
+      <c r="A120" s="1"/>
+      <c r="B120" t="s">
+        <v>169</v>
+      </c>
+      <c r="C120" t="s">
         <v>66</v>
       </c>
-      <c r="D117" t="s">
+      <c r="D120" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="118" spans="1:11">
-      <c r="A118" s="3"/>
-      <c r="B118" s="3"/>
-      <c r="C118" s="3"/>
-      <c r="D118" s="3"/>
-      <c r="E118" s="3"/>
-      <c r="F118" s="3"/>
-      <c r="G118" s="3"/>
-      <c r="H118" s="3"/>
-      <c r="I118" s="3"/>
-      <c r="J118" s="3"/>
-      <c r="K118" s="3"/>
-    </row>
-    <row r="119" spans="1:11">
-      <c r="A119" s="3"/>
-      <c r="B119" s="3"/>
-      <c r="C119" s="3"/>
-      <c r="D119" s="3"/>
-      <c r="E119" s="3"/>
-      <c r="F119" s="3"/>
-      <c r="G119" s="3"/>
-      <c r="H119" s="3"/>
-      <c r="I119" s="3"/>
-      <c r="J119" s="3"/>
-      <c r="K119" s="3"/>
-    </row>
-    <row r="120" spans="1:4">
-      <c r="A120" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="B120" t="s">
-        <v>167</v>
-      </c>
-      <c r="C120" t="s">
-        <v>70</v>
-      </c>
-      <c r="D120" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="121" spans="1:4">
-      <c r="A121" s="1"/>
-      <c r="B121" t="s">
-        <v>7</v>
-      </c>
-      <c r="C121" t="s">
-        <v>8</v>
-      </c>
-      <c r="D121" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="122" spans="1:4">
-      <c r="A122" s="1"/>
-      <c r="B122" t="s">
-        <v>169</v>
-      </c>
-      <c r="C122" t="s">
-        <v>70</v>
-      </c>
-      <c r="D122" t="s">
+    <row r="121" spans="1:11">
+      <c r="A121" s="3"/>
+      <c r="B121" s="3"/>
+      <c r="C121" s="3"/>
+      <c r="D121" s="3"/>
+      <c r="E121" s="3"/>
+      <c r="F121" s="3"/>
+      <c r="G121" s="3"/>
+      <c r="H121" s="3"/>
+      <c r="I121" s="3"/>
+      <c r="J121" s="3"/>
+      <c r="K121" s="3"/>
+    </row>
+    <row r="122" spans="1:11">
+      <c r="A122" s="3"/>
+      <c r="B122" s="3"/>
+      <c r="C122" s="3"/>
+      <c r="D122" s="3"/>
+      <c r="E122" s="3"/>
+      <c r="F122" s="3"/>
+      <c r="G122" s="3"/>
+      <c r="H122" s="3"/>
+      <c r="I122" s="3"/>
+      <c r="J122" s="3"/>
+      <c r="K122" s="3"/>
+    </row>
+    <row r="123" spans="1:4">
+      <c r="A123" s="1" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="123" spans="1:4">
-      <c r="A123" s="1"/>
       <c r="B123" t="s">
         <v>171</v>
       </c>
@@ -3104,60 +3116,96 @@
     <row r="124" spans="1:4">
       <c r="A124" s="1"/>
       <c r="B124" t="s">
-        <v>173</v>
+        <v>7</v>
       </c>
       <c r="C124" t="s">
-        <v>70</v>
+        <v>8</v>
       </c>
       <c r="D124" t="s">
-        <v>174</v>
+        <v>9</v>
       </c>
     </row>
     <row r="125" spans="1:4">
       <c r="A125" s="1"/>
       <c r="B125" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C125" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="D125" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="126" spans="1:4">
       <c r="A126" s="1"/>
       <c r="B126" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C126" t="s">
-        <v>8</v>
+        <v>70</v>
       </c>
       <c r="D126" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="127" spans="1:4">
       <c r="A127" s="1"/>
       <c r="B127" t="s">
+        <v>177</v>
+      </c>
+      <c r="C127" t="s">
+        <v>70</v>
+      </c>
+      <c r="D127" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4">
+      <c r="A128" s="1"/>
+      <c r="B128" t="s">
         <v>179</v>
       </c>
-      <c r="C127" t="s">
+      <c r="C128" t="s">
         <v>66</v>
       </c>
-      <c r="D127" t="s">
+      <c r="D128" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4">
+      <c r="A129" s="1"/>
+      <c r="B129" t="s">
+        <v>181</v>
+      </c>
+      <c r="C129" t="s">
+        <v>8</v>
+      </c>
+      <c r="D129" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4">
+      <c r="A130" s="1"/>
+      <c r="B130" t="s">
+        <v>183</v>
+      </c>
+      <c r="C130" t="s">
+        <v>66</v>
+      </c>
+      <c r="D130" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="128" spans="2:4">
-      <c r="B128" t="s">
-        <v>180</v>
-      </c>
-      <c r="C128" t="s">
+    <row r="131" spans="2:4">
+      <c r="B131" t="s">
+        <v>184</v>
+      </c>
+      <c r="C131" t="s">
         <v>70</v>
       </c>
-      <c r="D128" t="s">
-        <v>181</v>
+      <c r="D131" t="s">
+        <v>185</v>
       </c>
     </row>
   </sheetData>
@@ -3167,31 +3215,31 @@
     <mergeCell ref="A19:A22"/>
     <mergeCell ref="A25:A29"/>
     <mergeCell ref="A32:A36"/>
-    <mergeCell ref="A39:A47"/>
-    <mergeCell ref="A50:A52"/>
-    <mergeCell ref="A55:A63"/>
-    <mergeCell ref="A66:A73"/>
-    <mergeCell ref="A76:A78"/>
-    <mergeCell ref="A81:A88"/>
-    <mergeCell ref="A91:A100"/>
-    <mergeCell ref="A103:A108"/>
-    <mergeCell ref="A111:A116"/>
-    <mergeCell ref="A120:A127"/>
+    <mergeCell ref="A39:A50"/>
+    <mergeCell ref="A53:A55"/>
+    <mergeCell ref="A58:A66"/>
+    <mergeCell ref="A69:A76"/>
+    <mergeCell ref="A79:A81"/>
+    <mergeCell ref="A84:A91"/>
+    <mergeCell ref="A94:A103"/>
+    <mergeCell ref="A106:A111"/>
+    <mergeCell ref="A114:A119"/>
+    <mergeCell ref="A123:A130"/>
     <mergeCell ref="A1:E5"/>
     <mergeCell ref="A10:K11"/>
     <mergeCell ref="A17:K18"/>
     <mergeCell ref="A23:K24"/>
     <mergeCell ref="A30:K31"/>
     <mergeCell ref="A37:K38"/>
-    <mergeCell ref="A48:K49"/>
-    <mergeCell ref="A53:K54"/>
-    <mergeCell ref="A64:K65"/>
-    <mergeCell ref="A74:K75"/>
-    <mergeCell ref="A79:K80"/>
-    <mergeCell ref="A89:K90"/>
-    <mergeCell ref="A101:K102"/>
-    <mergeCell ref="A109:K110"/>
-    <mergeCell ref="A118:K119"/>
+    <mergeCell ref="A51:K52"/>
+    <mergeCell ref="A56:K57"/>
+    <mergeCell ref="A67:K68"/>
+    <mergeCell ref="A77:K78"/>
+    <mergeCell ref="A82:K83"/>
+    <mergeCell ref="A92:K93"/>
+    <mergeCell ref="A104:K105"/>
+    <mergeCell ref="A112:K113"/>
+    <mergeCell ref="A121:K122"/>
   </mergeCells>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
文档 Signed-off-by: LuoJhno <540088249@qq.com>
</commit_message>
<xml_diff>
--- a/毕业设计相关/数据库设计/实验教学平台_数据字典.xlsx
+++ b/毕业设计相关/数据库设计/实验教学平台_数据字典.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20385" windowHeight="8085"/>
+    <workbookView windowWidth="19665" windowHeight="6330"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222">
   <si>
     <t>实验教学管理平台_数据库表及字段</t>
   </si>
@@ -589,6 +589,99 @@
   </si>
   <si>
     <t>CSY162</t>
+  </si>
+  <si>
+    <t>AA10字典表</t>
+  </si>
+  <si>
+    <t>AAA100</t>
+  </si>
+  <si>
+    <t>代码类别</t>
+  </si>
+  <si>
+    <t>AAA101</t>
+  </si>
+  <si>
+    <t>代码总称</t>
+  </si>
+  <si>
+    <t>AAA102</t>
+  </si>
+  <si>
+    <t>代码码值</t>
+  </si>
+  <si>
+    <t>AAA103</t>
+  </si>
+  <si>
+    <t>代码名</t>
+  </si>
+  <si>
+    <t>AAA104</t>
+  </si>
+  <si>
+    <t>AAA105</t>
+  </si>
+  <si>
+    <t>备用字段</t>
+  </si>
+  <si>
+    <t>SY17日志表</t>
+  </si>
+  <si>
+    <t>CSY170</t>
+  </si>
+  <si>
+    <t>日志ID</t>
+  </si>
+  <si>
+    <t>CSY171</t>
+  </si>
+  <si>
+    <t>登陆ID</t>
+  </si>
+  <si>
+    <t>CSY172</t>
+  </si>
+  <si>
+    <t>访问程序</t>
+  </si>
+  <si>
+    <t>CSY173</t>
+  </si>
+  <si>
+    <t>IP地址</t>
+  </si>
+  <si>
+    <t>CSY174</t>
+  </si>
+  <si>
+    <t>时间</t>
+  </si>
+  <si>
+    <t>CSY175</t>
+  </si>
+  <si>
+    <t>浏览器信息</t>
+  </si>
+  <si>
+    <t>CSY176</t>
+  </si>
+  <si>
+    <t>访问系统信息</t>
+  </si>
+  <si>
+    <t>CSY177</t>
+  </si>
+  <si>
+    <t>主机名称</t>
+  </si>
+  <si>
+    <t>CSY178</t>
+  </si>
+  <si>
+    <t>mac地址</t>
   </si>
 </sst>
 </file>
@@ -618,14 +711,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -638,23 +731,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="宋体"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -668,6 +754,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
@@ -676,9 +770,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -689,6 +797,14 @@
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -710,22 +826,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -739,23 +847,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -782,13 +875,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -800,25 +923,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -830,7 +947,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -842,19 +959,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -872,13 +989,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -890,13 +1031,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -908,61 +1049,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -979,43 +1072,23 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1037,9 +1110,35 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1059,17 +1158,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1081,10 +1174,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1093,137 +1186,137 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="27" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="30" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1239,8 +1332,14 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1586,10 +1685,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:K136"/>
+  <dimension ref="A1:K155"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A116" workbookViewId="0">
-      <selection activeCell="E135" sqref="E135"/>
+    <sheetView tabSelected="1" topLeftCell="A136" workbookViewId="0">
+      <selection activeCell="D155" sqref="D155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -3248,7 +3347,7 @@
       <c r="D133" s="4"/>
     </row>
     <row r="134" spans="1:4">
-      <c r="A134" s="5" t="s">
+      <c r="A134" s="1" t="s">
         <v>186</v>
       </c>
       <c r="B134" t="s">
@@ -3262,7 +3361,7 @@
       </c>
     </row>
     <row r="135" spans="1:4">
-      <c r="A135" s="5"/>
+      <c r="A135" s="1"/>
       <c r="B135" t="s">
         <v>188</v>
       </c>
@@ -3274,7 +3373,7 @@
       </c>
     </row>
     <row r="136" spans="1:4">
-      <c r="A136" s="5"/>
+      <c r="A136" s="1"/>
       <c r="B136" t="s">
         <v>190</v>
       </c>
@@ -3285,8 +3384,214 @@
         <v>15</v>
       </c>
     </row>
+    <row r="137" spans="1:4">
+      <c r="A137" s="5"/>
+      <c r="B137" s="5"/>
+      <c r="C137" s="5"/>
+      <c r="D137" s="5"/>
+    </row>
+    <row r="138" spans="1:4">
+      <c r="A138" s="5"/>
+      <c r="B138" s="5"/>
+      <c r="C138" s="5"/>
+      <c r="D138" s="5"/>
+    </row>
+    <row r="139" spans="1:4">
+      <c r="A139" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="B139" t="s">
+        <v>192</v>
+      </c>
+      <c r="C139" t="s">
+        <v>37</v>
+      </c>
+      <c r="D139" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4">
+      <c r="A140" s="6"/>
+      <c r="B140" t="s">
+        <v>194</v>
+      </c>
+      <c r="C140" t="s">
+        <v>37</v>
+      </c>
+      <c r="D140" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4">
+      <c r="A141" s="6"/>
+      <c r="B141" t="s">
+        <v>196</v>
+      </c>
+      <c r="C141" t="s">
+        <v>37</v>
+      </c>
+      <c r="D141" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4">
+      <c r="A142" s="6"/>
+      <c r="B142" t="s">
+        <v>198</v>
+      </c>
+      <c r="C142" t="s">
+        <v>37</v>
+      </c>
+      <c r="D142" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4">
+      <c r="A143" s="6"/>
+      <c r="B143" t="s">
+        <v>200</v>
+      </c>
+      <c r="C143" t="s">
+        <v>66</v>
+      </c>
+      <c r="D143" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4">
+      <c r="A144" s="6"/>
+      <c r="B144" t="s">
+        <v>201</v>
+      </c>
+      <c r="C144" t="s">
+        <v>37</v>
+      </c>
+      <c r="D144" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4">
+      <c r="A145" s="7"/>
+      <c r="B145" s="7"/>
+      <c r="C145" s="7"/>
+      <c r="D145" s="7"/>
+    </row>
+    <row r="146" spans="1:4">
+      <c r="A146" s="7"/>
+      <c r="B146" s="7"/>
+      <c r="C146" s="7"/>
+      <c r="D146" s="7"/>
+    </row>
+    <row r="147" spans="1:4">
+      <c r="A147" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="B147" t="s">
+        <v>204</v>
+      </c>
+      <c r="C147" t="s">
+        <v>59</v>
+      </c>
+      <c r="D147" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4">
+      <c r="A148" s="6"/>
+      <c r="B148" t="s">
+        <v>206</v>
+      </c>
+      <c r="C148" t="s">
+        <v>37</v>
+      </c>
+      <c r="D148" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4">
+      <c r="A149" s="6"/>
+      <c r="B149" t="s">
+        <v>208</v>
+      </c>
+      <c r="C149" t="s">
+        <v>37</v>
+      </c>
+      <c r="D149" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4">
+      <c r="A150" s="6"/>
+      <c r="B150" t="s">
+        <v>210</v>
+      </c>
+      <c r="C150" t="s">
+        <v>37</v>
+      </c>
+      <c r="D150" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4">
+      <c r="A151" s="6"/>
+      <c r="B151" t="s">
+        <v>212</v>
+      </c>
+      <c r="C151" t="s">
+        <v>37</v>
+      </c>
+      <c r="D151" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4">
+      <c r="A152" s="6"/>
+      <c r="B152" t="s">
+        <v>214</v>
+      </c>
+      <c r="C152" t="s">
+        <v>37</v>
+      </c>
+      <c r="D152" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4">
+      <c r="A153" s="6"/>
+      <c r="B153" t="s">
+        <v>216</v>
+      </c>
+      <c r="C153" t="s">
+        <v>37</v>
+      </c>
+      <c r="D153" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="154" spans="2:4">
+      <c r="B154" t="s">
+        <v>218</v>
+      </c>
+      <c r="C154" t="s">
+        <v>37</v>
+      </c>
+      <c r="D154" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="155" spans="2:4">
+      <c r="B155" t="s">
+        <v>220</v>
+      </c>
+      <c r="C155" t="s">
+        <v>37</v>
+      </c>
+      <c r="D155" t="s">
+        <v>221</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="32">
+  <mergeCells count="35">
     <mergeCell ref="A7:A9"/>
     <mergeCell ref="A12:A16"/>
     <mergeCell ref="A19:A22"/>
@@ -3303,6 +3608,8 @@
     <mergeCell ref="A114:A119"/>
     <mergeCell ref="A123:A130"/>
     <mergeCell ref="A134:A136"/>
+    <mergeCell ref="A139:A144"/>
+    <mergeCell ref="A147:A153"/>
     <mergeCell ref="A1:E5"/>
     <mergeCell ref="A10:K11"/>
     <mergeCell ref="A17:K18"/>
@@ -3319,6 +3626,7 @@
     <mergeCell ref="A112:K113"/>
     <mergeCell ref="A121:K122"/>
     <mergeCell ref="A132:D133"/>
+    <mergeCell ref="A137:D138"/>
   </mergeCells>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>